<commit_message>
New Method for dictionary
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.dict.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3C9784-D5B4-9D47-A7BD-A63CD02E04FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4141A9E-BB72-B641-A2C9-DD49CF58D8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67020" yWindow="-6100" windowWidth="46400" windowHeight="27220" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22560" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-LDATA" sheetId="6" r:id="rId1"/>
@@ -731,7 +731,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A5" sqref="A5:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>

</xml_diff>

<commit_message>
Integration for Open Source
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.dict.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FDE9C9-D864-9147-B696-8D306DEFE827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63AAABE-4157-154F-AE14-315CE9B3705B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70580" yWindow="-2060" windowWidth="38400" windowHeight="22620" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="70580" yWindow="-7260" windowWidth="38400" windowHeight="27800" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-LDATA" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="144">
   <si>
     <t>code</t>
   </si>
@@ -268,10 +268,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开源接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ftp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -284,10 +280,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>open.source</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>eaae9d54-0a22-4d7f-b714-b8c236d607f8</t>
   </si>
   <si>
@@ -432,54 +424,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>zero.attachment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>普通附件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合同附件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文件管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>凭证单据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FILE.REQUEST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FILE.CONTRACT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FILE.COMMON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FILE.CREDIT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>48352a99-7abf-4772-8ccc-5c1d56bf0db2</t>
-  </si>
-  <si>
-    <t>8f709cb1-6ce3-4614-a7b7-ad3df1af5fa9</t>
-  </si>
-  <si>
-    <t>62428f80-5e9a-4c3c-b440-c9091b6c2394</t>
-  </si>
-  <si>
-    <t>302ba2f5-05b8-4133-8a92-8dd7c0778e42</t>
-  </si>
-  <si>
     <t>zero.tabular</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -589,6 +533,14 @@
   <si>
     <t>vendor</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三方接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>os</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1092,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B153567-C702-204F-B537-960DCAAE5957}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -1415,7 +1367,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="8" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>24</v>
@@ -1424,10 +1376,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -1495,7 +1447,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>39</v>
@@ -1507,7 +1459,7 @@
         <v>64</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -1515,7 +1467,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>39</v>
@@ -1524,10 +1476,10 @@
         <v>3</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
@@ -1535,7 +1487,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>65</v>
@@ -1547,7 +1499,7 @@
         <v>67</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23"/>
       <c r="G23"/>
@@ -1555,7 +1507,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>65</v>
@@ -1567,7 +1519,7 @@
         <v>66</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24"/>
       <c r="G24"/>
@@ -1575,7 +1527,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>65</v>
@@ -1587,7 +1539,7 @@
         <v>68</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25"/>
       <c r="G25"/>
@@ -1595,7 +1547,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>65</v>
@@ -1604,10 +1556,10 @@
         <v>4</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="F26"/>
       <c r="G26"/>
@@ -1615,19 +1567,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27"/>
       <c r="G27"/>
@@ -1635,19 +1587,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="5">
         <v>2</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F28"/>
       <c r="G28"/>
@@ -1655,19 +1607,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C29" s="5">
         <v>3</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F29"/>
       <c r="G29"/>
@@ -1675,19 +1627,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30" s="5">
         <v>4</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F30"/>
       <c r="G30"/>
@@ -1695,19 +1647,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="5">
         <v>5</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F31"/>
       <c r="G31"/>
@@ -1715,19 +1667,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C32" s="5">
         <v>6</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F32"/>
       <c r="G32"/>
@@ -1735,19 +1687,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" s="5">
         <v>7</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F33"/>
       <c r="G33"/>
@@ -1755,19 +1707,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" s="5">
         <v>8</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F34"/>
       <c r="G34"/>
@@ -1775,19 +1727,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="5">
         <v>9</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F35"/>
       <c r="G35"/>
@@ -1795,19 +1747,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36" s="5">
         <v>10</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F36"/>
       <c r="G36"/>
@@ -1815,19 +1767,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C37" s="5">
         <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F37"/>
       <c r="G37"/>
@@ -1835,16 +1787,16 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C38" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>121</v>
@@ -1855,19 +1807,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C39" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F39"/>
       <c r="G39"/>
@@ -1875,19 +1827,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C40" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F40"/>
       <c r="G40"/>
@@ -1895,19 +1847,19 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C41" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F41"/>
       <c r="G41"/>
@@ -1915,133 +1867,53 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="8" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C42" s="5">
         <v>1</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
+        <v>131</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="8" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C43" s="5">
         <v>2</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
+        <v>132</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C44" s="5">
         <v>3</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C45" s="5">
-        <v>4</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45"/>
-      <c r="G45"/>
-      <c r="H45"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C46" s="5">
-        <v>1</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" s="5">
-        <v>2</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C48" s="5">
-        <v>3</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>